<commit_message>
Setup new housing dictionary
</commit_message>
<xml_diff>
--- a/pricing-by-area-new.xlsx
+++ b/pricing-by-area-new.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6A7A910-082A-4DFF-A303-B9A162B267A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="23250" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="23250" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New-property-area-ann" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Malcolm Hillis - (DECLG)</author>
   </authors>
   <commentList>
-    <comment ref="B48" authorId="0">
+    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H48" authorId="0">
+    <comment ref="H48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -52,67 +64,67 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
-    <t>The most current data is published on these sheets. Previously published data may be subject to revision. Any change from the originally published data will be highlighted by a comment on the cell in question. These comments will be maintained for at least a year after the date of the value change.</t>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>Annual New Property prices  (includes houses and apartments) €</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>Cork</t>
+  </si>
+  <si>
+    <t>Galway</t>
+  </si>
+  <si>
+    <t>Limerick</t>
+  </si>
+  <si>
+    <t>Waterford</t>
+  </si>
+  <si>
+    <t>Other Areas</t>
+  </si>
+  <si>
+    <t>1969/70</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>1970/71</t>
+  </si>
+  <si>
+    <t>1971/72</t>
+  </si>
+  <si>
+    <t>1972/73</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior to 1974 the data was based on surveys of existing house sales in Dublin carried out  by  the Valuation Office on behalf of the D. O. E. Since 1974 the data has been based on information supplied by all lending agencies on the average price of mortgage financed existing house transactions. </t>
+  </si>
+  <si>
+    <t>Average house prices are derived from data supplied by the mortgage lending agencies on loans approved by them rather than loans paid. In comparing house prices figures from one period to another, account should be taken of the fact that changes in the mix of houses (incl apartments) will affect the average figures.</t>
   </si>
   <si>
     <t>Data for 1969/1970 is not available for Cork, Limerick, Galway, Waterford and Other areas</t>
   </si>
   <si>
-    <t>Average house prices are derived from data supplied by the mortgage lending agencies on loans approved by them rather than loans paid. In comparing house prices figures from one period to another, account should be taken of the fact that changes in the mix of houses (incl apartments) will affect the average figures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prior to 1974 the data was based on surveys of existing house sales in Dublin carried out  by  the Valuation Office on behalf of the D. O. E. Since 1974 the data has been based on information supplied by all lending agencies on the average price of mortgage financed existing house transactions. </t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>1972/73</t>
-  </si>
-  <si>
-    <t>1971/72</t>
-  </si>
-  <si>
-    <t>1970/71</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>1969/70</t>
-  </si>
-  <si>
-    <t>Other Areas</t>
-  </si>
-  <si>
-    <t>Waterford</t>
-  </si>
-  <si>
-    <t>Limerick</t>
-  </si>
-  <si>
-    <t>Galway</t>
-  </si>
-  <si>
-    <t>Cork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dublin </t>
-  </si>
-  <si>
-    <t>National</t>
-  </si>
-  <si>
-    <t>Annual New Property prices  (includes houses and apartments) €</t>
-  </si>
-  <si>
-    <t>YEAR</t>
+    <t>The most current data is published on these sheets. Previously published data may be subject to revision. Any change from the originally published data will be highlighted by a comment on the cell in question. These comments will be maintained for at least a year after the date of the value change.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -412,9 +424,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -475,6 +484,9 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -498,20 +510,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Comma 2" xfId="1"/>
-    <cellStyle name="Comma 3" xfId="2"/>
-    <cellStyle name="Currency 2" xfId="3"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Normal 4" xfId="6"/>
-    <cellStyle name="Normal 5" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -560,7 +575,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,9 +608,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,6 +660,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -803,14 +852,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A53" sqref="A53:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" customHeight="1"/>
@@ -825,10 +874,10 @@
   <sheetData>
     <row r="1" spans="1:9" thickBot="1">
       <c r="A1" s="34" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
@@ -839,650 +888,650 @@
     </row>
     <row r="2" spans="1:9" thickBot="1">
       <c r="A2" s="35"/>
-      <c r="B2" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="B2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1">
+      <c r="A3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>6691.5196733217872</v>
+      </c>
+      <c r="C3" s="14">
+        <v>7050.855549517245</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1">
+      <c r="A4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="14">
+        <v>7523.1981146929011</v>
+      </c>
+      <c r="C4" s="14">
+        <v>7913.0077047706591</v>
+      </c>
+      <c r="D4" s="14">
+        <v>6631.8419836356152</v>
+      </c>
+      <c r="E4" s="14">
+        <v>6975.9410028899238</v>
+      </c>
+      <c r="F4" s="14">
+        <v>6012.2098013621744</v>
+      </c>
+      <c r="G4" s="14">
+        <v>6104.9006810875053</v>
+      </c>
+      <c r="H4" s="13">
+        <v>6427.4141530085171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1">
+      <c r="A5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="14">
+        <v>8249.4882955543926</v>
+      </c>
+      <c r="C5" s="14">
+        <v>8527.5609347303835</v>
+      </c>
+      <c r="D5" s="14">
+        <v>7675.5666841044022</v>
+      </c>
+      <c r="E5" s="14">
+        <v>8866.5810016709747</v>
+      </c>
+      <c r="F5" s="14">
+        <v>6733.4210299099495</v>
+      </c>
+      <c r="G5" s="14">
+        <v>6226.7955366167062</v>
+      </c>
+      <c r="H5" s="13">
+        <v>7198.1451666150306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1">
-      <c r="A3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="15">
-        <v>6691.5196733217872</v>
-      </c>
-      <c r="C3" s="15">
-        <v>7050.855549517245</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="15">
-        <v>7523.1981146929011</v>
-      </c>
-      <c r="C4" s="15">
-        <v>7913.0077047706591</v>
-      </c>
-      <c r="D4" s="15">
-        <v>6631.8419836356152</v>
-      </c>
-      <c r="E4" s="15">
-        <v>6975.9410028899238</v>
-      </c>
-      <c r="F4" s="15">
-        <v>6012.2098013621744</v>
-      </c>
-      <c r="G4" s="15">
-        <v>6104.9006810875053</v>
-      </c>
-      <c r="H4" s="14">
-        <v>6427.4141530085171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="15">
-        <v>8249.4882955543926</v>
-      </c>
-      <c r="C5" s="15">
-        <v>8527.5609347303835</v>
-      </c>
-      <c r="D5" s="15">
-        <v>7675.5666841044022</v>
-      </c>
-      <c r="E5" s="15">
-        <v>8866.5810016709747</v>
-      </c>
-      <c r="F5" s="15">
-        <v>6733.4210299099495</v>
-      </c>
-      <c r="G5" s="15">
-        <v>6226.7955366167062</v>
-      </c>
-      <c r="H5" s="14">
-        <v>7198.1451666150306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1">
-      <c r="A6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>9008.791666455043</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>9205.601068611566</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>7678.1061602612608</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>9404.9499469249477</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>7449.5533061440083</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="14">
         <v>6927.6909559096148</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>8053.9486314762989</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>1974</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>10835.944761314635</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>10942.602759902687</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>9808.7266558654283</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>13356.374846996561</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>10514.701027472052</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>9571.2856351991704</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>10851.181618255785</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>1975</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>13253.526062643798</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>13136.710159428312</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>12920.854686095352</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>14420.415356720216</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>13593.815867662817</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>12636.433356527215</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>13832.526626407503</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>1976</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>15564.449365384908</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>15342.2452016598</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>15347.324153973517</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>17842.359478086859</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>15278.758297738341</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>13899.82274456425</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>15361.291272836239</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>1977</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>18754.031418399012</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>19054.959342986727</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>18652.452372124677</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>21715.060617295861</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <v>19992.026044867463</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <v>17296.372104362312</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>18025.20176138066</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>1978</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>24081.852395487858</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>25745.209278230086</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>22460.396869333792</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>26244.216343052754</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <v>23077.489575450374</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <v>21294.777313335802</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>22838.77881670569</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>1979</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>29386.818087164978</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>32005.018004885951</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>29064.304615243967</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>30466.095453829781</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <v>30538.470524300246</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <v>27163.506711835482</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>27136.842212188469</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>1980</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>34967.316941861231</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>37821.688142170031</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>34616.869232214776</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>33838.519790137689</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>34340.066331117217</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <v>32135.801026964156</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <v>32662.742329512268</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>1981</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>40166.894373028728</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>44456.069601962503</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>35463.784530527038</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>39728.83473597066</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>41520.43516463424</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="14">
         <v>34638.454779548076</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="13">
         <v>37857.240808366048</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1">
-      <c r="A15" s="16">
+      <c r="A15" s="15">
         <v>1982</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>44059.911321492604</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>48886.185757601917</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>38212.767470326216</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>45460.432421999991</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>40194.828610754172</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <v>41741.369590280912</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="13">
         <v>42889.212813180893</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>1983</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>44448.451173491929</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>48168.78374328943</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>39223.478980755848</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>45649.623395685936</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>41430.283761065766</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="14">
         <v>42132.448918437105</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <v>43501.226566983758</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="18" customHeight="1">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>1984</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>45418.531065411822</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>48818.889639445173</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>41105.230812987895</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>45774.057727371997</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>42943.81155055335</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="14">
         <v>44114.510058865053</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="13">
         <v>43653.595136395263</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="18" customHeight="1">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>1985</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>46542.24926482165</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>49165.528134856337</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>42738.113981847819</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <v>49004.271398895835</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>44510.668339334959</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="14">
         <v>43741.207063806876</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <v>45057.92545113794</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1">
-      <c r="A19" s="16">
+      <c r="A19" s="15">
         <v>1986</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>48256.395670701044</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>50891.102183441595</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <v>43844.055848159638</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="14">
         <v>49804.206388306215</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <v>47221.559136781259</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="14">
         <v>47927.533508387889</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="13">
         <v>46486.380789370764</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="18" customHeight="1">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>1987</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>48151.007410191422</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>50864.437683794582</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="14">
         <v>45846.432797842455</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="14">
         <v>48162.435052897286</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="14">
         <v>46946.025973762131</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="14">
         <v>46966.341783017</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <v>45739.77479925441</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="18" customHeight="1">
-      <c r="A21" s="16">
+      <c r="A21" s="15">
         <v>1988</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>52450.340543752631</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>57994.016994174439</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <v>49604.857509992835</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>52238.294284654956</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <v>53295.98610398647</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="14">
         <v>47531.375227917983</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="13">
         <v>47380.276396584908</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="18" customHeight="1">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <v>1989</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>58178.12901554667</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <v>68393.171856509434</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="14">
         <v>54669.842704846844</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="14">
         <v>57935.609042566699</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="14">
         <v>54732.059870689875</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="14">
         <v>50506.371545677554</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="13">
         <v>51354.556582068246</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="18" customHeight="1">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <v>1990</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>65541.340132357494</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>80748.993097703802</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="14">
         <v>61074.401572443632</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="14">
         <v>68018.599123372827</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="14">
         <v>62257.797461539631</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="14">
         <v>53904.190643554044</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H23" s="13">
         <v>55728.804262256781</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="18" customHeight="1">
-      <c r="A24" s="16">
+      <c r="A24" s="15">
         <v>1991</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>66913.926995139438</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <v>78714.872696060251</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="14">
         <v>64651.253739378641</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="14">
         <v>66784.413711139656</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="14">
         <v>64597.924740084614</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="14">
         <v>53365.821698300075</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="13">
         <v>58645.392628408612</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="18" customHeight="1">
-      <c r="A25" s="16">
+      <c r="A25" s="15">
         <v>1992</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>69264.212178311849</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <v>79199.912642020194</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="14">
         <v>65107.089709534717</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>75417.362906379669</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="14">
         <v>60184.315179464778</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="14">
         <v>52656.038112458162</v>
       </c>
-      <c r="H25" s="14">
+      <c r="H25" s="13">
         <v>62433.021316362858</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="18" customHeight="1">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>1993</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>69882.574622506872</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>75539.25776190887</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="14">
         <v>68172.237430862762</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="14">
         <v>74760.908319831782</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <v>66825.045329649394</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="14">
         <v>61341.046568913764</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="13">
         <v>65024.556734436817</v>
       </c>
       <c r="J26" s="3"/>
@@ -1492,760 +1541,760 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="16">
+      <c r="A27" s="15">
         <v>1994</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <v>72731.866870501952</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>81993.336414564401</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="14">
         <v>71378.32607889644</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="14">
         <v>77375.299023317464</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="14">
         <v>68238.263810941076</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="14">
         <v>69185.488417449247</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="13">
         <v>66828.854543884678</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="16">
+      <c r="A28" s="15">
         <v>1995</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>77993.661467512473</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <v>86671.051495497508</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="14">
         <v>76608.377223946241</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="14">
         <v>87783.342052201464</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="14">
         <v>73347.6898385401</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="14">
         <v>69949.870740663609</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="13">
         <v>71829.083096738803</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="16">
+      <c r="A29" s="15">
         <v>1996</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>87201.802012280896</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <v>97057.508977048215</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="14">
         <v>85350.523893931153</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="14">
         <v>93050.215601525706</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="14">
         <v>83280.850826091584</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="14">
         <v>79783.992158097622</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="13">
         <v>82091.106246603449</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="16">
+      <c r="A30" s="15">
         <v>1997</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>102221.53374201969</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <v>122035.79645590707</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="14">
         <v>96045.527728540153</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="14">
         <v>109904.71885459467</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="14">
         <v>91077.042627646762</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="14">
         <v>91607.793144430165</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="13">
         <v>94664.052699209205</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="16">
+      <c r="A31" s="15">
         <v>1998</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>125301.56279362693</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>160699.32094407565</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="14">
         <v>112133.10918223788</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="14">
         <v>118738.28666622649</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="14">
         <v>104248.03571519266</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="14">
         <v>107954.40116612744</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="13">
         <v>116588.62009944588</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="16">
+      <c r="A32" s="15">
         <v>1999</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="14">
         <v>148521.26303386138</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="14">
         <v>193525.85948570527</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="14">
         <v>141006.95308571748</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="14">
         <v>138928.3918513289</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="14">
         <v>121879.61867226027</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="14">
         <v>132050.22068047803</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="13">
         <v>136970.45573439111</v>
       </c>
     </row>
     <row r="33" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="16">
+      <c r="A33" s="15">
         <v>2000</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>169191</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>221724</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="14">
         <v>166557</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="14">
         <v>163824</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="14">
         <v>145834</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="14">
         <v>145713</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="13">
         <v>154050</v>
       </c>
     </row>
     <row r="34" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A34" s="16">
+      <c r="A34" s="15">
         <v>2001</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="14">
         <v>182863</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="14">
         <v>243095</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="14">
         <v>174550</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="14">
         <v>171161</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="14">
         <v>152205</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G34" s="14">
         <v>155488</v>
       </c>
-      <c r="H34" s="14">
+      <c r="H34" s="13">
         <v>166834</v>
       </c>
     </row>
     <row r="35" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="16">
+      <c r="A35" s="15">
         <v>2002</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="14">
         <v>198087</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="14">
         <v>256109</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="14">
         <v>184369</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="14">
         <v>187607</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="14">
         <v>168574</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="14">
         <v>167272</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H35" s="13">
         <v>179936</v>
       </c>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
     </row>
     <row r="36" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A36" s="16">
+      <c r="A36" s="15">
         <v>2003</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="14">
         <v>224567</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="14">
         <v>291646</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="14">
         <v>211980</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="14">
         <v>223388</v>
       </c>
-      <c r="F36" s="15">
+      <c r="F36" s="14">
         <v>197672</v>
       </c>
-      <c r="G36" s="15">
+      <c r="G36" s="14">
         <v>195173</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="13">
         <v>203125</v>
       </c>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
-      <c r="AB36" s="13"/>
-      <c r="AC36" s="13"/>
-      <c r="AD36" s="13"/>
-      <c r="AE36" s="13"/>
-      <c r="AF36" s="13"/>
-      <c r="AG36" s="13"/>
-      <c r="AH36" s="13"/>
-      <c r="AI36" s="13"/>
-      <c r="AJ36" s="13"/>
-      <c r="AK36" s="13"/>
-      <c r="AL36" s="13"/>
-      <c r="AM36" s="13"/>
-      <c r="AN36" s="13"/>
-      <c r="AO36" s="13"/>
-      <c r="AP36" s="13"/>
-      <c r="AQ36" s="13"/>
-      <c r="AR36" s="13"/>
-      <c r="AS36" s="13"/>
-      <c r="AT36" s="13"/>
-      <c r="AU36" s="13"/>
-      <c r="AV36" s="13"/>
-      <c r="AW36" s="13"/>
-      <c r="AX36" s="13"/>
-      <c r="AY36" s="13"/>
-      <c r="AZ36" s="13"/>
-      <c r="BA36" s="13"/>
-      <c r="BB36" s="13"/>
-      <c r="BC36" s="13"/>
-      <c r="BD36" s="13"/>
-      <c r="BE36" s="13"/>
-      <c r="BF36" s="13"/>
-      <c r="BG36" s="13"/>
-      <c r="BH36" s="13"/>
-      <c r="BI36" s="13"/>
-      <c r="BJ36" s="13"/>
-      <c r="BK36" s="13"/>
-      <c r="BL36" s="13"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="12"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="12"/>
+      <c r="AC36" s="12"/>
+      <c r="AD36" s="12"/>
+      <c r="AE36" s="12"/>
+      <c r="AF36" s="12"/>
+      <c r="AG36" s="12"/>
+      <c r="AH36" s="12"/>
+      <c r="AI36" s="12"/>
+      <c r="AJ36" s="12"/>
+      <c r="AK36" s="12"/>
+      <c r="AL36" s="12"/>
+      <c r="AM36" s="12"/>
+      <c r="AN36" s="12"/>
+      <c r="AO36" s="12"/>
+      <c r="AP36" s="12"/>
+      <c r="AQ36" s="12"/>
+      <c r="AR36" s="12"/>
+      <c r="AS36" s="12"/>
+      <c r="AT36" s="12"/>
+      <c r="AU36" s="12"/>
+      <c r="AV36" s="12"/>
+      <c r="AW36" s="12"/>
+      <c r="AX36" s="12"/>
+      <c r="AY36" s="12"/>
+      <c r="AZ36" s="12"/>
+      <c r="BA36" s="12"/>
+      <c r="BB36" s="12"/>
+      <c r="BC36" s="12"/>
+      <c r="BD36" s="12"/>
+      <c r="BE36" s="12"/>
+      <c r="BF36" s="12"/>
+      <c r="BG36" s="12"/>
+      <c r="BH36" s="12"/>
+      <c r="BI36" s="12"/>
+      <c r="BJ36" s="12"/>
+      <c r="BK36" s="12"/>
+      <c r="BL36" s="12"/>
     </row>
     <row r="37" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A37" s="16">
+      <c r="A37" s="15">
         <v>2004</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="14">
         <v>249191</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="14">
         <v>322628</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="14">
         <v>237858</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="14">
         <v>242218</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F37" s="14">
         <v>210868</v>
       </c>
-      <c r="G37" s="15">
+      <c r="G37" s="14">
         <v>220286</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H37" s="13">
         <v>228057</v>
       </c>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
-      <c r="T37" s="13"/>
-      <c r="U37" s="13"/>
-      <c r="V37" s="13"/>
-      <c r="W37" s="13"/>
-      <c r="X37" s="13"/>
-      <c r="Y37" s="13"/>
-      <c r="Z37" s="13"/>
-      <c r="AA37" s="13"/>
-      <c r="AB37" s="13"/>
-      <c r="AC37" s="13"/>
-      <c r="AD37" s="13"/>
-      <c r="AE37" s="13"/>
-      <c r="AF37" s="13"/>
-      <c r="AG37" s="13"/>
-      <c r="AH37" s="13"/>
-      <c r="AI37" s="13"/>
-      <c r="AJ37" s="13"/>
-      <c r="AK37" s="13"/>
-      <c r="AL37" s="13"/>
-      <c r="AM37" s="13"/>
-      <c r="AN37" s="13"/>
-      <c r="AO37" s="13"/>
-      <c r="AP37" s="13"/>
-      <c r="AQ37" s="13"/>
-      <c r="AR37" s="13"/>
-      <c r="AS37" s="13"/>
-      <c r="AT37" s="13"/>
-      <c r="AU37" s="13"/>
-      <c r="AV37" s="13"/>
-      <c r="AW37" s="13"/>
-      <c r="AX37" s="13"/>
-      <c r="AY37" s="13"/>
-      <c r="AZ37" s="13"/>
-      <c r="BA37" s="13"/>
-      <c r="BB37" s="13"/>
-      <c r="BC37" s="13"/>
-      <c r="BD37" s="13"/>
-      <c r="BE37" s="13"/>
-      <c r="BF37" s="13"/>
-      <c r="BG37" s="13"/>
-      <c r="BH37" s="13"/>
-      <c r="BI37" s="13"/>
-      <c r="BJ37" s="13"/>
-      <c r="BK37" s="13"/>
-      <c r="BL37" s="13"/>
-      <c r="BM37" s="13"/>
-      <c r="BN37" s="13"/>
-      <c r="BO37" s="13"/>
-      <c r="BP37" s="13"/>
-      <c r="BQ37" s="13"/>
-      <c r="BR37" s="13"/>
-      <c r="BS37" s="13"/>
-      <c r="BT37" s="13"/>
-      <c r="BU37" s="13"/>
-      <c r="BV37" s="13"/>
-      <c r="BW37" s="13"/>
-      <c r="BX37" s="13"/>
-      <c r="BY37" s="13"/>
-      <c r="BZ37" s="13"/>
-      <c r="CA37" s="13"/>
-      <c r="CB37" s="13"/>
-      <c r="CC37" s="13"/>
-      <c r="CD37" s="13"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="12"/>
+      <c r="V37" s="12"/>
+      <c r="W37" s="12"/>
+      <c r="X37" s="12"/>
+      <c r="Y37" s="12"/>
+      <c r="Z37" s="12"/>
+      <c r="AA37" s="12"/>
+      <c r="AB37" s="12"/>
+      <c r="AC37" s="12"/>
+      <c r="AD37" s="12"/>
+      <c r="AE37" s="12"/>
+      <c r="AF37" s="12"/>
+      <c r="AG37" s="12"/>
+      <c r="AH37" s="12"/>
+      <c r="AI37" s="12"/>
+      <c r="AJ37" s="12"/>
+      <c r="AK37" s="12"/>
+      <c r="AL37" s="12"/>
+      <c r="AM37" s="12"/>
+      <c r="AN37" s="12"/>
+      <c r="AO37" s="12"/>
+      <c r="AP37" s="12"/>
+      <c r="AQ37" s="12"/>
+      <c r="AR37" s="12"/>
+      <c r="AS37" s="12"/>
+      <c r="AT37" s="12"/>
+      <c r="AU37" s="12"/>
+      <c r="AV37" s="12"/>
+      <c r="AW37" s="12"/>
+      <c r="AX37" s="12"/>
+      <c r="AY37" s="12"/>
+      <c r="AZ37" s="12"/>
+      <c r="BA37" s="12"/>
+      <c r="BB37" s="12"/>
+      <c r="BC37" s="12"/>
+      <c r="BD37" s="12"/>
+      <c r="BE37" s="12"/>
+      <c r="BF37" s="12"/>
+      <c r="BG37" s="12"/>
+      <c r="BH37" s="12"/>
+      <c r="BI37" s="12"/>
+      <c r="BJ37" s="12"/>
+      <c r="BK37" s="12"/>
+      <c r="BL37" s="12"/>
+      <c r="BM37" s="12"/>
+      <c r="BN37" s="12"/>
+      <c r="BO37" s="12"/>
+      <c r="BP37" s="12"/>
+      <c r="BQ37" s="12"/>
+      <c r="BR37" s="12"/>
+      <c r="BS37" s="12"/>
+      <c r="BT37" s="12"/>
+      <c r="BU37" s="12"/>
+      <c r="BV37" s="12"/>
+      <c r="BW37" s="12"/>
+      <c r="BX37" s="12"/>
+      <c r="BY37" s="12"/>
+      <c r="BZ37" s="12"/>
+      <c r="CA37" s="12"/>
+      <c r="CB37" s="12"/>
+      <c r="CC37" s="12"/>
+      <c r="CD37" s="12"/>
     </row>
     <row r="38" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A38" s="16">
+      <c r="A38" s="15">
         <v>2005</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="14">
         <v>276221</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="14">
         <v>350891</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="14">
         <v>265644</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="14">
         <v>274905</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="14">
         <v>226393</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="14">
         <v>246914</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="13">
         <v>254006</v>
       </c>
     </row>
     <row r="39" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A39" s="16">
+      <c r="A39" s="15">
         <v>2006</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="14">
         <v>305637</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="14">
         <v>405957</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="14">
         <v>305015</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="14">
         <v>286176</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F39" s="14">
         <v>275411</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G39" s="14">
         <v>271521</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="13">
         <v>276570</v>
       </c>
     </row>
     <row r="40" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A40" s="16">
+      <c r="A40" s="15">
         <v>2007</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="14">
         <v>322634</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="14">
         <v>416225</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="14">
         <v>325453</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="14">
         <v>300750</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="14">
         <v>288202</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G40" s="14">
         <v>292057</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="13">
         <v>296605</v>
       </c>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-    </row>
-    <row r="41" spans="1:82" s="13" customFormat="1" ht="18" customHeight="1">
-      <c r="A41" s="16">
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+    </row>
+    <row r="41" spans="1:82" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A41" s="15">
         <v>2008</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="14">
         <v>305269</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="14">
         <v>370495</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="14">
         <v>314276</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="14">
         <v>292777</v>
       </c>
-      <c r="F41" s="15">
+      <c r="F41" s="14">
         <v>276719</v>
       </c>
-      <c r="G41" s="15">
+      <c r="G41" s="14">
         <v>288478</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="13">
         <v>282677</v>
       </c>
     </row>
     <row r="42" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A42" s="16">
+      <c r="A42" s="15">
         <v>2009</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="14">
         <v>242033</v>
       </c>
-      <c r="C42" s="15">
+      <c r="C42" s="14">
         <v>260170</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="14">
         <v>252011</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="14">
         <v>236113</v>
       </c>
-      <c r="F42" s="15">
+      <c r="F42" s="14">
         <v>260684</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G42" s="14">
         <v>227444</v>
       </c>
-      <c r="H42" s="14">
+      <c r="H42" s="13">
         <v>231739</v>
       </c>
     </row>
-    <row r="43" spans="1:82" s="13" customFormat="1" ht="18" customHeight="1">
-      <c r="A43" s="16">
+    <row r="43" spans="1:82" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A43" s="15">
         <v>2010</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="14">
         <v>228268</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="14">
         <v>251629</v>
       </c>
-      <c r="D43" s="15">
+      <c r="D43" s="14">
         <v>244333</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="14">
         <v>219459</v>
       </c>
-      <c r="F43" s="15">
+      <c r="F43" s="14">
         <v>224778</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G43" s="14">
         <v>224021</v>
       </c>
-      <c r="H43" s="14">
+      <c r="H43" s="13">
         <v>218097</v>
       </c>
     </row>
-    <row r="44" spans="1:82" s="13" customFormat="1" ht="18" customHeight="1">
-      <c r="A44" s="16">
+    <row r="44" spans="1:82" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A44" s="15">
         <v>2011</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="14">
         <v>230303</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="14">
         <v>290668</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="14">
         <v>241502</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="14">
         <v>229558</v>
       </c>
-      <c r="F44" s="15">
+      <c r="F44" s="14">
         <v>216307</v>
       </c>
-      <c r="G44" s="15">
+      <c r="G44" s="14">
         <v>205598</v>
       </c>
-      <c r="H44" s="14">
+      <c r="H44" s="13">
         <v>216400</v>
       </c>
     </row>
     <row r="45" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A45" s="16">
+      <c r="A45" s="15">
         <v>2012</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="14">
         <v>220415</v>
       </c>
-      <c r="C45" s="15">
+      <c r="C45" s="14">
         <v>265633</v>
       </c>
-      <c r="D45" s="15">
+      <c r="D45" s="14">
         <v>235473</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="14">
         <v>219233</v>
       </c>
-      <c r="F45" s="15">
+      <c r="F45" s="14">
         <v>212902</v>
       </c>
-      <c r="G45" s="15">
+      <c r="G45" s="14">
         <v>179716</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45" s="13">
         <v>207957</v>
       </c>
     </row>
     <row r="46" spans="1:82" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A46" s="16">
+      <c r="A46" s="15">
         <v>2013</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="14">
         <v>228216</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="14">
         <v>300466</v>
       </c>
-      <c r="D46" s="15">
+      <c r="D46" s="14">
         <v>240063</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="14">
         <v>218308</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="14">
         <v>206456</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="14">
         <v>154051</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H46" s="13">
         <v>207573</v>
       </c>
     </row>
-    <row r="47" spans="1:82" s="13" customFormat="1" ht="18" customHeight="1">
-      <c r="A47" s="21">
+    <row r="47" spans="1:82" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A47" s="20">
         <v>2014</v>
       </c>
-      <c r="B47" s="22">
+      <c r="B47" s="21">
         <v>246378</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="21">
         <v>333720</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="21">
         <v>242099</v>
       </c>
-      <c r="E47" s="22">
+      <c r="E47" s="21">
         <v>218016</v>
       </c>
-      <c r="F47" s="22">
+      <c r="F47" s="21">
         <v>208442</v>
       </c>
-      <c r="G47" s="22">
+      <c r="G47" s="21">
         <v>177122</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="13">
         <v>214404</v>
       </c>
     </row>
-    <row r="48" spans="1:82" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A48" s="26">
+    <row r="48" spans="1:82" s="12" customFormat="1" ht="18" customHeight="1" thickBot="1">
+      <c r="A48" s="25">
         <v>2015</v>
       </c>
-      <c r="B48" s="27">
+      <c r="B48" s="26">
         <v>281432</v>
       </c>
-      <c r="C48" s="27">
+      <c r="C48" s="26">
         <v>377741</v>
       </c>
-      <c r="D48" s="27">
+      <c r="D48" s="26">
         <v>255010</v>
       </c>
-      <c r="E48" s="27">
+      <c r="E48" s="26">
         <v>241058</v>
       </c>
-      <c r="F48" s="27">
+      <c r="F48" s="26">
         <v>232791</v>
       </c>
-      <c r="G48" s="27">
+      <c r="G48" s="26">
         <v>213506</v>
       </c>
-      <c r="H48" s="28">
+      <c r="H48" s="27">
         <v>251437</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="23.45" customHeight="1" thickBot="1">
-      <c r="A49" s="23">
+      <c r="A49" s="22">
         <v>2016</v>
       </c>
-      <c r="B49" s="24">
+      <c r="B49" s="23">
         <v>313483</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="23">
         <v>397676</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="23">
         <v>293343</v>
       </c>
-      <c r="E49" s="24">
+      <c r="E49" s="23">
         <v>262215</v>
       </c>
-      <c r="F49" s="24">
+      <c r="F49" s="23">
         <v>239024</v>
       </c>
-      <c r="G49" s="24">
+      <c r="G49" s="23">
         <v>239409</v>
       </c>
-      <c r="H49" s="25">
+      <c r="H49" s="24">
         <v>272290</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15.75">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="9"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="8"/>
     </row>
     <row r="51" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A51" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="9"/>
+      <c r="A51" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="8"/>
     </row>
     <row r="52" spans="1:14" ht="30.75" customHeight="1">
       <c r="A52" s="30" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
@@ -2257,7 +2306,7 @@
     </row>
     <row r="53" spans="1:14" ht="15.75">
       <c r="A53" s="30" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -2268,11 +2317,11 @@
       <c r="H53" s="30"/>
     </row>
     <row r="54" spans="1:14" ht="32.25" customHeight="1">
-      <c r="A54" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -2281,7 +2330,7 @@
     </row>
     <row r="55" spans="1:14" ht="34.5" customHeight="1">
       <c r="A55" s="29" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="29"/>

</xml_diff>